<commit_message>
revisions finished, need to proof, fixes #16, #17
</commit_message>
<xml_diff>
--- a/data-raw/swfwmdrainfall.xlsx
+++ b/data-raw/swfwmdrainfall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Users\DCB\E_Walters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://swfwmd-my.sharepoint.com/personal/erin_walters_swfwmd_state_fl_us/Documents/APRILrain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DA020D9-88A2-4706-BF8E-227B7A79C775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{82CCEA04-5AAC-4433-A7DC-69AB8258648F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A78C74D4-607C-45C3-BEDB-F26F4456ACE4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" tabRatio="961" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jan-usgsbsn" sheetId="1" r:id="rId1"/>
@@ -32,16 +32,16 @@
     <sheet name="ESRI_MAPINFO_SHEET" sheetId="17" state="veryHidden" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="ann_usgsbasin" localSheetId="12">'ann-usgsbsn'!$A$1:$N$114</definedName>
-    <definedName name="apr_usgsbasin" localSheetId="3">'apr-usgsbsn'!$A$1:$N$114</definedName>
+    <definedName name="ann_usgsbasin" localSheetId="12">'ann-usgsbsn'!$A$1:$N$115</definedName>
+    <definedName name="apr_usgsbasin" localSheetId="3">'apr-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="aug_usgsbasin" localSheetId="7">'aug-usgsbsn'!$A$1:$N$114</definedName>
     <definedName name="dec_usgsbasin" localSheetId="11">'dec-usgsbsn'!$A$1:$N$114</definedName>
     <definedName name="dry_usgsbasin" localSheetId="14">'dry-usgsbsn'!$A$1:$N$115</definedName>
-    <definedName name="feb_usgsbasin" localSheetId="1">'feb-usgsbsn'!$A$1:$N$114</definedName>
-    <definedName name="jan_usgsbasin" localSheetId="0">'jan-usgsbsn'!$A$1:$N$114</definedName>
+    <definedName name="feb_usgsbasin" localSheetId="1">'feb-usgsbsn'!$A$1:$N$115</definedName>
+    <definedName name="jan_usgsbasin" localSheetId="0">'jan-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="jul_usgsbasin" localSheetId="6">'jul-usgsbsn'!$A$1:$N$114</definedName>
     <definedName name="jun_usgsbasin" localSheetId="5">'jun-usgsbsn'!$A$1:$N$114</definedName>
-    <definedName name="mar_usgsbasin" localSheetId="2">'mar-usgsbsn'!$A$1:$N$114</definedName>
+    <definedName name="mar_usgsbasin" localSheetId="2">'mar-usgsbsn'!$A$1:$N$115</definedName>
     <definedName name="may_usgsbasin" localSheetId="4">'may-usgsbsn'!$A$1:$N$114</definedName>
     <definedName name="nov_usgsbasin" localSheetId="10">'nov-usgsbsn'!$A$1:$N$114</definedName>
     <definedName name="oct_usgsbasin" localSheetId="9">'oct-usgsbsn'!$A$1:$N$114</definedName>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="34">
   <si>
     <t>January Rainfall Summary Data by USGS Drainage Basin</t>
   </si>
@@ -1033,29 +1033,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O114"/>
+  <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="43.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5997,134 +5997,178 @@
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
-        <v>15</v>
+      <c r="A112" s="2">
+        <v>2024</v>
       </c>
       <c r="B112" s="3">
-        <v>0.06</v>
+        <v>3.57</v>
       </c>
       <c r="C112" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="D112" s="3">
-        <v>0</v>
+        <v>2.89</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E112" s="3">
-        <v>0.03</v>
+        <v>2.63</v>
       </c>
       <c r="F112" s="3">
-        <v>0</v>
+        <v>3.69</v>
       </c>
       <c r="G112" s="3">
-        <v>0</v>
+        <v>2.83</v>
       </c>
       <c r="H112" s="3">
-        <v>0.03</v>
+        <v>4.07</v>
       </c>
       <c r="I112" s="3">
-        <v>0.06</v>
+        <v>3.38</v>
       </c>
       <c r="J112" s="3">
-        <v>0.05</v>
+        <v>2.83</v>
       </c>
       <c r="K112" s="3">
-        <v>0</v>
+        <v>3.37</v>
       </c>
       <c r="L112" s="3">
-        <v>0</v>
+        <v>3.26</v>
       </c>
       <c r="M112" s="3">
-        <v>0</v>
+        <v>4.12</v>
       </c>
       <c r="N112" s="3">
-        <v>0</v>
+        <v>4.58</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B113" s="3">
-        <v>3.02</v>
+        <v>0.06</v>
       </c>
       <c r="C113" s="3">
-        <v>2.61</v>
+        <v>0.02</v>
       </c>
       <c r="D113" s="3">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="E113" s="3">
-        <v>2.5299999999999998</v>
+        <v>0.03</v>
       </c>
       <c r="F113" s="3">
-        <v>2.13</v>
+        <v>0</v>
       </c>
       <c r="G113" s="3">
-        <v>2.41</v>
+        <v>0</v>
       </c>
       <c r="H113" s="3">
-        <v>2.14</v>
+        <v>0.03</v>
       </c>
       <c r="I113" s="3">
-        <v>2.39</v>
+        <v>0.06</v>
       </c>
       <c r="J113" s="3">
-        <v>2.42</v>
+        <v>0.05</v>
       </c>
       <c r="K113" s="3">
-        <v>2.41</v>
+        <v>0</v>
       </c>
       <c r="L113" s="3">
-        <v>2.3199999999999998</v>
+        <v>0</v>
       </c>
       <c r="M113" s="3">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="N113" s="3">
-        <v>2.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" s="3">
+        <v>3.02</v>
+      </c>
+      <c r="C114" s="3">
+        <v>2.62</v>
+      </c>
+      <c r="D114" s="3">
+        <v>2.78</v>
+      </c>
+      <c r="E114" s="3">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="F114" s="3">
+        <v>2.15</v>
+      </c>
+      <c r="G114" s="3">
+        <v>2.42</v>
+      </c>
+      <c r="H114" s="3">
+        <v>2.16</v>
+      </c>
+      <c r="I114" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="J114" s="3">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="K114" s="3">
+        <v>2.42</v>
+      </c>
+      <c r="L114" s="3">
+        <v>2.33</v>
+      </c>
+      <c r="M114" s="3">
+        <v>2.21</v>
+      </c>
+      <c r="N114" s="3">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B115" s="3">
         <v>10.76</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C115" s="3">
         <v>7.39</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D115" s="3">
         <v>7.45</v>
       </c>
-      <c r="E114" s="3">
+      <c r="E115" s="3">
         <v>7.52</v>
       </c>
-      <c r="F114" s="3">
+      <c r="F115" s="3">
         <v>7.57</v>
       </c>
-      <c r="G114" s="3">
+      <c r="G115" s="3">
         <v>8.0299999999999994</v>
       </c>
-      <c r="H114" s="3">
+      <c r="H115" s="3">
         <v>7.69</v>
       </c>
-      <c r="I114" s="3">
+      <c r="I115" s="3">
         <v>7.99</v>
       </c>
-      <c r="J114" s="3">
+      <c r="J115" s="3">
         <v>8.02</v>
       </c>
-      <c r="K114" s="3">
+      <c r="K115" s="3">
         <v>8.08</v>
       </c>
-      <c r="L114" s="3">
+      <c r="L115" s="3">
         <v>8.64</v>
       </c>
-      <c r="M114" s="3">
+      <c r="M115" s="3">
         <v>7.63</v>
       </c>
-      <c r="N114" s="3">
+      <c r="N115" s="3">
         <v>10.51</v>
       </c>
     </row>
@@ -6145,23 +6189,23 @@
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="43.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -11249,23 +11293,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -16441,27 +16485,27 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -21635,29 +21679,29 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:O114"/>
+  <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="51.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -26599,134 +26643,178 @@
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B112" s="3">
-        <v>31.96</v>
-      </c>
-      <c r="C112" s="3">
-        <v>32.08</v>
-      </c>
-      <c r="D112" s="3">
-        <v>37.840000000000003</v>
-      </c>
-      <c r="E112" s="3">
-        <v>31.42</v>
-      </c>
-      <c r="F112" s="3">
-        <v>28.75</v>
-      </c>
-      <c r="G112" s="3">
-        <v>33.43</v>
-      </c>
-      <c r="H112" s="3">
-        <v>30.72</v>
-      </c>
-      <c r="I112" s="3">
-        <v>33.229999999999997</v>
-      </c>
-      <c r="J112" s="3">
-        <v>35.25</v>
-      </c>
-      <c r="K112" s="3">
-        <v>31.66</v>
-      </c>
-      <c r="L112" s="3">
-        <v>30.19</v>
-      </c>
-      <c r="M112" s="3">
-        <v>37.24</v>
-      </c>
-      <c r="N112" s="3">
-        <v>30.03</v>
+      <c r="A112" s="2">
+        <v>2024</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M112" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N112" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B113" s="3">
-        <v>54.13</v>
+        <v>31.96</v>
       </c>
       <c r="C113" s="3">
-        <v>52.89</v>
+        <v>32.08</v>
       </c>
       <c r="D113" s="3">
-        <v>54.37</v>
+        <v>37.840000000000003</v>
       </c>
       <c r="E113" s="3">
-        <v>53.65</v>
+        <v>31.42</v>
       </c>
       <c r="F113" s="3">
-        <v>51.97</v>
+        <v>28.75</v>
       </c>
       <c r="G113" s="3">
-        <v>51.62</v>
+        <v>33.43</v>
       </c>
       <c r="H113" s="3">
-        <v>52.12</v>
+        <v>30.72</v>
       </c>
       <c r="I113" s="3">
-        <v>52.54</v>
+        <v>33.229999999999997</v>
       </c>
       <c r="J113" s="3">
-        <v>52.88</v>
+        <v>35.25</v>
       </c>
       <c r="K113" s="3">
-        <v>53.45</v>
+        <v>31.66</v>
       </c>
       <c r="L113" s="3">
-        <v>51.65</v>
+        <v>30.19</v>
       </c>
       <c r="M113" s="3">
-        <v>53.18</v>
+        <v>37.24</v>
       </c>
       <c r="N113" s="3">
-        <v>51.27</v>
+        <v>30.03</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" s="3">
+        <v>54.13</v>
+      </c>
+      <c r="C114" s="3">
+        <v>52.89</v>
+      </c>
+      <c r="D114" s="3">
+        <v>54.37</v>
+      </c>
+      <c r="E114" s="3">
+        <v>53.65</v>
+      </c>
+      <c r="F114" s="3">
+        <v>51.97</v>
+      </c>
+      <c r="G114" s="3">
+        <v>51.62</v>
+      </c>
+      <c r="H114" s="3">
+        <v>52.12</v>
+      </c>
+      <c r="I114" s="3">
+        <v>52.54</v>
+      </c>
+      <c r="J114" s="3">
+        <v>52.88</v>
+      </c>
+      <c r="K114" s="3">
+        <v>53.45</v>
+      </c>
+      <c r="L114" s="3">
+        <v>51.65</v>
+      </c>
+      <c r="M114" s="3">
+        <v>53.18</v>
+      </c>
+      <c r="N114" s="3">
+        <v>51.27</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B115" s="3">
         <v>78.72</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C115" s="3">
         <v>76.819999999999993</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D115" s="3">
         <v>78.38</v>
       </c>
-      <c r="E114" s="3">
+      <c r="E115" s="3">
         <v>77.66</v>
       </c>
-      <c r="F114" s="3">
+      <c r="F115" s="3">
         <v>75.88</v>
       </c>
-      <c r="G114" s="3">
+      <c r="G115" s="3">
         <v>82.14</v>
       </c>
-      <c r="H114" s="3">
+      <c r="H115" s="3">
         <v>77.849999999999994</v>
       </c>
-      <c r="I114" s="3">
+      <c r="I115" s="3">
         <v>77.78</v>
       </c>
-      <c r="J114" s="3">
+      <c r="J115" s="3">
         <v>81.45</v>
       </c>
-      <c r="K114" s="3">
+      <c r="K115" s="3">
         <v>87.44</v>
       </c>
-      <c r="L114" s="3">
+      <c r="L115" s="3">
         <v>85.54</v>
       </c>
-      <c r="M114" s="3">
+      <c r="M115" s="3">
         <v>80.41</v>
       </c>
-      <c r="N114" s="3">
+      <c r="N115" s="3">
         <v>88.1</v>
       </c>
     </row>
@@ -26746,23 +26834,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="61.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -31846,27 +31934,27 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="58" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -36905,43 +36993,43 @@
         <v>2024</v>
       </c>
       <c r="B112" s="3">
-        <v>11.46</v>
+        <v>23.99</v>
       </c>
       <c r="C112" s="3">
-        <v>9.84</v>
+        <v>21.54</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E112" s="3">
-        <v>7.37</v>
+        <v>17.87</v>
       </c>
       <c r="F112" s="3">
-        <v>5.78</v>
+        <v>14.41</v>
       </c>
       <c r="G112" s="3">
-        <v>6.01</v>
+        <v>16.18</v>
       </c>
       <c r="H112" s="3">
-        <v>5.71</v>
+        <v>14.72</v>
       </c>
       <c r="I112" s="3">
-        <v>5.61</v>
+        <v>15.61</v>
       </c>
       <c r="J112" s="3">
-        <v>5.21</v>
+        <v>13.81</v>
       </c>
       <c r="K112" s="3">
-        <v>4.57</v>
+        <v>13.59</v>
       </c>
       <c r="L112" s="3">
-        <v>5.16</v>
+        <v>13.82</v>
       </c>
       <c r="M112" s="3">
-        <v>4.75</v>
+        <v>14.01</v>
       </c>
       <c r="N112" s="3">
-        <v>8.33</v>
+        <v>18.48</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
@@ -36952,37 +37040,37 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="C113" s="3">
-        <v>9.84</v>
+        <v>10.92</v>
       </c>
       <c r="D113" s="3">
         <v>1.84</v>
       </c>
       <c r="E113" s="3">
-        <v>7.37</v>
+        <v>10.29</v>
       </c>
       <c r="F113" s="3">
-        <v>5.78</v>
+        <v>9.16</v>
       </c>
       <c r="G113" s="3">
-        <v>6.01</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="H113" s="3">
-        <v>5.71</v>
+        <v>9.82</v>
       </c>
       <c r="I113" s="3">
-        <v>5.61</v>
+        <v>10.46</v>
       </c>
       <c r="J113" s="3">
-        <v>5.21</v>
+        <v>9.5399999999999991</v>
       </c>
       <c r="K113" s="3">
-        <v>4.57</v>
+        <v>9.31</v>
       </c>
       <c r="L113" s="3">
-        <v>5.16</v>
+        <v>7.85</v>
       </c>
       <c r="M113" s="3">
-        <v>4.75</v>
+        <v>6.64</v>
       </c>
       <c r="N113" s="3">
         <v>6.25</v>
@@ -36993,43 +37081,43 @@
         <v>16</v>
       </c>
       <c r="B114" s="3">
-        <v>24.47</v>
+        <v>24.58</v>
       </c>
       <c r="C114" s="3">
-        <v>22.77</v>
+        <v>22.88</v>
       </c>
       <c r="D114" s="3">
         <v>22.99</v>
       </c>
       <c r="E114" s="3">
-        <v>22.23</v>
+        <v>22.33</v>
       </c>
       <c r="F114" s="3">
-        <v>20.95</v>
+        <v>21.03</v>
       </c>
       <c r="G114" s="3">
-        <v>20.63</v>
+        <v>20.72</v>
       </c>
       <c r="H114" s="3">
-        <v>20.46</v>
+        <v>20.54</v>
       </c>
       <c r="I114" s="3">
-        <v>21.31</v>
+        <v>21.4</v>
       </c>
       <c r="J114" s="3">
-        <v>20.86</v>
+        <v>20.94</v>
       </c>
       <c r="K114" s="3">
-        <v>20.45</v>
+        <v>20.53</v>
       </c>
       <c r="L114" s="3">
-        <v>20.100000000000001</v>
+        <v>20.18</v>
       </c>
       <c r="M114" s="3">
-        <v>20.010000000000002</v>
+        <v>20.09</v>
       </c>
       <c r="N114" s="3">
-        <v>19.28</v>
+        <v>19.37</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
@@ -37092,23 +37180,23 @@
       <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="63.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -42348,7 +42436,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -42358,29 +42446,29 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O114"/>
+  <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.44140625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="6.42578125" style="1"/>
+    <col min="1" max="1" width="44.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="6.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -47322,134 +47410,178 @@
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
-        <v>15</v>
+      <c r="A112" s="2">
+        <v>2024</v>
       </c>
       <c r="B112" s="3">
-        <v>0.48</v>
+        <v>2.83</v>
       </c>
       <c r="C112" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="D112" s="3">
-        <v>0.4</v>
+        <v>3.45</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E112" s="3">
-        <v>0.23</v>
+        <v>3.01</v>
       </c>
       <c r="F112" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>2.02</v>
       </c>
       <c r="G112" s="3">
-        <v>0.12</v>
+        <v>3.07</v>
       </c>
       <c r="H112" s="3">
-        <v>0.09</v>
+        <v>2.15</v>
       </c>
       <c r="I112" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="J112" s="3">
-        <v>0.04</v>
+        <v>2.6</v>
       </c>
       <c r="K112" s="3">
-        <v>0.02</v>
+        <v>3.43</v>
       </c>
       <c r="L112" s="3">
-        <v>0.02</v>
+        <v>2.95</v>
       </c>
       <c r="M112" s="3">
-        <v>0.01</v>
+        <v>2.54</v>
       </c>
       <c r="N112" s="3">
-        <v>0</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B113" s="3">
-        <v>3.23</v>
+        <v>0.48</v>
       </c>
       <c r="C113" s="3">
-        <v>2.84</v>
+        <v>0.26</v>
       </c>
       <c r="D113" s="3">
-        <v>2.99</v>
+        <v>0.4</v>
       </c>
       <c r="E113" s="3">
-        <v>2.84</v>
+        <v>0.23</v>
       </c>
       <c r="F113" s="3">
-        <v>2.4700000000000002</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G113" s="3">
-        <v>2.74</v>
+        <v>0.12</v>
       </c>
       <c r="H113" s="3">
-        <v>2.44</v>
+        <v>0.09</v>
       </c>
       <c r="I113" s="3">
-        <v>2.73</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J113" s="3">
-        <v>2.73</v>
+        <v>0.04</v>
       </c>
       <c r="K113" s="3">
-        <v>2.67</v>
+        <v>0.02</v>
       </c>
       <c r="L113" s="3">
-        <v>2.52</v>
+        <v>0.02</v>
       </c>
       <c r="M113" s="3">
-        <v>2.4500000000000002</v>
+        <v>0.01</v>
       </c>
       <c r="N113" s="3">
-        <v>2.21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" s="3">
+        <v>3.22</v>
+      </c>
+      <c r="C114" s="3">
+        <v>2.84</v>
+      </c>
+      <c r="D114" s="3">
+        <v>2.99</v>
+      </c>
+      <c r="E114" s="3">
+        <v>2.84</v>
+      </c>
+      <c r="F114" s="3">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="G114" s="3">
+        <v>2.74</v>
+      </c>
+      <c r="H114" s="3">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="I114" s="3">
+        <v>2.73</v>
+      </c>
+      <c r="J114" s="3">
+        <v>2.72</v>
+      </c>
+      <c r="K114" s="3">
+        <v>2.68</v>
+      </c>
+      <c r="L114" s="3">
+        <v>2.52</v>
+      </c>
+      <c r="M114" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N114" s="3">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B115" s="3">
         <v>10.46</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C115" s="3">
         <v>9.25</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D115" s="3">
         <v>11.08</v>
       </c>
-      <c r="E114" s="3">
+      <c r="E115" s="3">
         <v>9.7799999999999994</v>
       </c>
-      <c r="F114" s="3">
+      <c r="F115" s="3">
         <v>9.74</v>
       </c>
-      <c r="G114" s="3">
+      <c r="G115" s="3">
         <v>10.49</v>
       </c>
-      <c r="H114" s="3">
+      <c r="H115" s="3">
         <v>9.92</v>
       </c>
-      <c r="I114" s="3">
+      <c r="I115" s="3">
         <v>10.48</v>
       </c>
-      <c r="J114" s="3">
+      <c r="J115" s="3">
         <v>10.87</v>
       </c>
-      <c r="K114" s="3">
+      <c r="K115" s="3">
         <v>9.5</v>
       </c>
-      <c r="L114" s="3">
+      <c r="L115" s="3">
         <v>9.34</v>
       </c>
-      <c r="M114" s="3">
+      <c r="M115" s="3">
         <v>9.52</v>
       </c>
-      <c r="N114" s="3">
+      <c r="N115" s="3">
         <v>12.11</v>
       </c>
     </row>
@@ -47464,29 +47596,29 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:P114"/>
+  <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="42.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -52522,134 +52654,178 @@
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A112" s="6" t="s">
-        <v>15</v>
+      <c r="A112" s="6">
+        <v>2024</v>
       </c>
       <c r="B112" s="3">
-        <v>0.16</v>
+        <v>3.9</v>
       </c>
       <c r="C112" s="3">
-        <v>0.08</v>
-      </c>
-      <c r="D112" s="3">
-        <v>0.11</v>
+        <v>3.56</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E112" s="3">
-        <v>0.05</v>
+        <v>3.34</v>
       </c>
       <c r="F112" s="3">
-        <v>0.16</v>
+        <v>1.91</v>
       </c>
       <c r="G112" s="3">
-        <v>0.05</v>
+        <v>2.7</v>
       </c>
       <c r="H112" s="3">
-        <v>0.2</v>
+        <v>1.78</v>
       </c>
       <c r="I112" s="3">
-        <v>0.22</v>
+        <v>2.65</v>
       </c>
       <c r="J112" s="3">
-        <v>0.05</v>
+        <v>1.6</v>
       </c>
       <c r="K112" s="3">
-        <v>0.06</v>
+        <v>1.18</v>
       </c>
       <c r="L112" s="3">
-        <v>0.08</v>
+        <v>1.57</v>
       </c>
       <c r="M112" s="3">
-        <v>0.09</v>
+        <v>1.67</v>
       </c>
       <c r="N112" s="3">
-        <v>0</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B113" s="3">
-        <v>3.84</v>
+        <v>0.16</v>
       </c>
       <c r="C113" s="3">
-        <v>3.7</v>
+        <v>0.08</v>
       </c>
       <c r="D113" s="3">
-        <v>3.92</v>
+        <v>0.11</v>
       </c>
       <c r="E113" s="3">
-        <v>3.49</v>
+        <v>0.05</v>
       </c>
       <c r="F113" s="3">
-        <v>2.9</v>
+        <v>0.16</v>
       </c>
       <c r="G113" s="3">
-        <v>3.2</v>
+        <v>0.05</v>
       </c>
       <c r="H113" s="3">
-        <v>2.84</v>
+        <v>0.2</v>
       </c>
       <c r="I113" s="3">
-        <v>3.14</v>
+        <v>0.22</v>
       </c>
       <c r="J113" s="3">
-        <v>3.01</v>
+        <v>0.05</v>
       </c>
       <c r="K113" s="3">
-        <v>2.97</v>
+        <v>0.06</v>
       </c>
       <c r="L113" s="3">
-        <v>2.89</v>
+        <v>0.08</v>
       </c>
       <c r="M113" s="3">
-        <v>2.76</v>
+        <v>0.09</v>
       </c>
       <c r="N113" s="3">
-        <v>2.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" s="3">
+        <v>3.84</v>
+      </c>
+      <c r="C114" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="D114" s="3">
+        <v>3.92</v>
+      </c>
+      <c r="E114" s="3">
+        <v>3.49</v>
+      </c>
+      <c r="F114" s="3">
+        <v>2.89</v>
+      </c>
+      <c r="G114" s="3">
+        <v>3.19</v>
+      </c>
+      <c r="H114" s="3">
+        <v>2.83</v>
+      </c>
+      <c r="I114" s="3">
+        <v>3.14</v>
+      </c>
+      <c r="J114" s="3">
+        <v>3</v>
+      </c>
+      <c r="K114" s="3">
+        <v>2.96</v>
+      </c>
+      <c r="L114" s="3">
+        <v>2.88</v>
+      </c>
+      <c r="M114" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="N114" s="3">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A115" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B115" s="3">
         <v>12.13</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C115" s="3">
         <v>14.87</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D115" s="3">
         <v>15.39</v>
       </c>
-      <c r="E114" s="3">
+      <c r="E115" s="3">
         <v>14.24</v>
       </c>
-      <c r="F114" s="3">
+      <c r="F115" s="3">
         <v>8.52</v>
       </c>
-      <c r="G114" s="3">
+      <c r="G115" s="3">
         <v>12.87</v>
       </c>
-      <c r="H114" s="3">
+      <c r="H115" s="3">
         <v>8.11</v>
       </c>
-      <c r="I114" s="3">
+      <c r="I115" s="3">
         <v>10.64</v>
       </c>
-      <c r="J114" s="3">
+      <c r="J115" s="3">
         <v>11.1</v>
       </c>
-      <c r="K114" s="3">
+      <c r="K115" s="3">
         <v>10.01</v>
       </c>
-      <c r="L114" s="3">
+      <c r="L115" s="3">
         <v>10.56</v>
       </c>
-      <c r="M114" s="3">
+      <c r="M115" s="3">
         <v>10.050000000000001</v>
       </c>
-      <c r="N114" s="3">
+      <c r="N115" s="3">
         <v>9.91</v>
       </c>
     </row>
@@ -52663,29 +52839,29 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N114"/>
+  <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="41.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -57534,134 +57710,178 @@
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
-        <v>15</v>
+      <c r="A112" s="2">
+        <v>2024</v>
       </c>
       <c r="B112" s="3">
-        <v>0.11</v>
+        <v>2.23</v>
       </c>
       <c r="C112" s="3">
-        <v>0</v>
-      </c>
-      <c r="D112" s="3">
-        <v>0</v>
+        <v>1.8</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E112" s="3">
-        <v>0</v>
+        <v>1.52</v>
       </c>
       <c r="F112" s="3">
-        <v>0.11</v>
+        <v>1.01</v>
       </c>
       <c r="G112" s="3">
-        <v>0</v>
+        <v>1.57</v>
       </c>
       <c r="H112" s="3">
-        <v>0.06</v>
+        <v>1.01</v>
       </c>
       <c r="I112" s="3">
-        <v>0.01</v>
+        <v>1.71</v>
       </c>
       <c r="J112" s="3">
-        <v>0</v>
+        <v>1.57</v>
       </c>
       <c r="K112" s="3">
-        <v>0</v>
+        <v>1.04</v>
       </c>
       <c r="L112" s="3">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="M112" s="3">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="N112" s="3">
-        <v>0</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B113" s="3">
-        <v>3.09</v>
+        <v>0.11</v>
       </c>
       <c r="C113" s="3">
-        <v>2.75</v>
+        <v>0</v>
       </c>
       <c r="D113" s="3">
-        <v>2.64</v>
+        <v>0</v>
       </c>
       <c r="E113" s="3">
-        <v>2.64</v>
+        <v>0</v>
       </c>
       <c r="F113" s="3">
-        <v>2.65</v>
+        <v>0.11</v>
       </c>
       <c r="G113" s="3">
-        <v>2.39</v>
+        <v>0</v>
       </c>
       <c r="H113" s="3">
-        <v>2.5499999999999998</v>
+        <v>0.06</v>
       </c>
       <c r="I113" s="3">
-        <v>2.56</v>
+        <v>0.01</v>
       </c>
       <c r="J113" s="3">
-        <v>2.46</v>
+        <v>0</v>
       </c>
       <c r="K113" s="3">
-        <v>2.46</v>
+        <v>0</v>
       </c>
       <c r="L113" s="3">
-        <v>2.4300000000000002</v>
+        <v>0</v>
       </c>
       <c r="M113" s="3">
-        <v>2.42</v>
+        <v>0</v>
       </c>
       <c r="N113" s="3">
-        <v>2.2200000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" s="3">
+        <v>3.09</v>
+      </c>
+      <c r="C114" s="3">
+        <v>2.74</v>
+      </c>
+      <c r="D114" s="3">
+        <v>2.64</v>
+      </c>
+      <c r="E114" s="3">
+        <v>2.63</v>
+      </c>
+      <c r="F114" s="3">
+        <v>2.63</v>
+      </c>
+      <c r="G114" s="3">
+        <v>2.38</v>
+      </c>
+      <c r="H114" s="3">
+        <v>2.54</v>
+      </c>
+      <c r="I114" s="3">
+        <v>2.56</v>
+      </c>
+      <c r="J114" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="K114" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="L114" s="3">
+        <v>2.41</v>
+      </c>
+      <c r="M114" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="N114" s="3">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B115" s="3">
         <v>9.4</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C115" s="3">
         <v>10.63</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D115" s="3">
         <v>10.48</v>
       </c>
-      <c r="E114" s="3">
+      <c r="E115" s="3">
         <v>8.31</v>
       </c>
-      <c r="F114" s="3">
+      <c r="F115" s="3">
         <v>7.77</v>
       </c>
-      <c r="G114" s="3">
+      <c r="G115" s="3">
         <v>8.15</v>
       </c>
-      <c r="H114" s="3">
+      <c r="H115" s="3">
         <v>7.57</v>
       </c>
-      <c r="I114" s="3">
+      <c r="I115" s="3">
         <v>10.25</v>
       </c>
-      <c r="J114" s="3">
+      <c r="J115" s="3">
         <v>9.85</v>
       </c>
-      <c r="K114" s="3">
+      <c r="K115" s="3">
         <v>9.81</v>
       </c>
-      <c r="L114" s="3">
+      <c r="L115" s="3">
         <v>12.31</v>
       </c>
-      <c r="M114" s="3">
+      <c r="M115" s="3">
         <v>8.17</v>
       </c>
-      <c r="N114" s="3">
+      <c r="N115" s="3">
         <v>8.6999999999999993</v>
       </c>
     </row>
@@ -57680,23 +57900,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="40.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -62875,23 +63095,23 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="41.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -70462,23 +70682,23 @@
       <selection activeCell="A73" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="40.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -75565,23 +75785,23 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="43.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -80669,23 +80889,23 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="46.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>